<commit_message>
Excel Read value using Iterator function updated
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginTest.xlsx
+++ b/src/test/resources/LoginTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumPractice\NigalyaHandsON\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8095773-15CD-4634-931D-7BB49ED282F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9B97E7-EE28-45B2-A9FD-4070520841E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Approved</t>
   </si>
   <si>
-    <t>auap@bd.com</t>
-  </si>
-  <si>
     <t>Deloitte@123</t>
   </si>
   <si>
@@ -61,6 +58,18 @@
   </si>
   <si>
     <t>CartCount</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>QALive</t>
   </si>
 </sst>
 </file>
@@ -390,76 +399,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.08984375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
+      <c r="E1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>4.0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{ABD323A4-580C-44E9-AB0D-49854A2607C4}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{3CACB520-A45E-41F6-9018-023725C37F54}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{72F326A2-0D29-4EC3-9474-39D53EB198BC}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{E7F4849C-11B3-4BC8-B45C-082205155EEF}"/>
-    <hyperlink ref="A4" r:id="rId5" xr:uid="{ACC9230C-7926-4235-875D-6037AAA15855}"/>
-    <hyperlink ref="B4" r:id="rId6" xr:uid="{7FA4E7DA-1459-4F38-B421-1E5DB3D1C4F2}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{ABD323A4-580C-44E9-AB0D-49854A2607C4}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{3CACB520-A45E-41F6-9018-023725C37F54}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{72F326A2-0D29-4EC3-9474-39D53EB198BC}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{E7F4849C-11B3-4BC8-B45C-082205155EEF}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{ACC9230C-7926-4235-875D-6037AAA15855}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{7FA4E7DA-1459-4F38-B421-1E5DB3D1C4F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>